<commit_message>
Up for getting multiple 'processos'
</commit_message>
<xml_diff>
--- a/data/outputs/analysis_summary.xlsx
+++ b/data/outputs/analysis_summary.xlsx
@@ -478,27 +478,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>08804604000100</t>
+          <t>43213049000135</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AVOHAI EVENTOS LTDA</t>
+          <t>RHAIANY SOARES SILVA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>169.000,00</t>
+          <t>14707320767</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SME-PRO-2025/27598</t>
+          <t>TUR-PRO-2025/01056</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://acesso.processo.rio/sigaex/public/app/transparencia/processo?n=SME-PRO-2025/27598</t>
+          <t>https://acesso.processo.rio/sigaex/public/app/transparencia/processo?n=TUR-PRO-2025/01056</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-12-29T14:38:47.201965</t>
+          <t>2025-12-29T16:57:53.530794</t>
         </is>
       </c>
     </row>

</xml_diff>